<commit_message>
Final testing report added
</commit_message>
<xml_diff>
--- a/Documentation/Test_Plan.xlsx
+++ b/Documentation/Test_Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d_tay\Documents\GitHub\Group27_Tracker\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BAA6ADE-E379-4BAD-AA31-D2B6147F858F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8FD308-0AF3-48C3-8610-AC20B3F0669F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" activeTab="1" xr2:uid="{02453E8A-D2D6-4E39-A09F-A8CC1B9D2C64}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{02453E8A-D2D6-4E39-A09F-A8CC1B9D2C64}"/>
   </bookViews>
   <sheets>
     <sheet name="Device Tests" sheetId="1" r:id="rId1"/>
@@ -357,9 +357,6 @@
     <t>Samples not available for testing</t>
   </si>
   <si>
-    <t>Attach Device by Velcro pad to each sample from &lt;step&gt;</t>
-  </si>
-  <si>
     <t>Device attaches to each sample</t>
   </si>
   <si>
@@ -526,6 +523,9 @@
   </si>
   <si>
     <t>Email appears in the mailbox of the registered user with a battery warning</t>
+  </si>
+  <si>
+    <t>Attach Device by Velcro pad to each sample from 1.42</t>
   </si>
 </sst>
 </file>
@@ -894,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C84F29F-14D0-4E66-89A4-E61AD12D137F}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,6 +1234,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <f t="shared" si="0"/>
+        <v>1.1900000000000002</v>
+      </c>
       <c r="B21" s="1" t="s">
         <v>94</v>
       </c>
@@ -1245,14 +1249,18 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2000000000000002</v>
+      </c>
       <c r="B22" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <f>A20+0.01</f>
-        <v>1.1900000000000002</v>
+        <f t="shared" si="0"/>
+        <v>1.2100000000000002</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>91</v>
@@ -1261,7 +1269,7 @@
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <f t="shared" si="0"/>
-        <v>1.2000000000000002</v>
+        <v>1.2200000000000002</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>92</v>
@@ -1270,7 +1278,7 @@
     <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <f t="shared" si="0"/>
-        <v>1.2100000000000002</v>
+        <v>1.2300000000000002</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>97</v>
@@ -1291,7 +1299,7 @@
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <f t="shared" si="0"/>
-        <v>1.2200000000000002</v>
+        <v>1.2400000000000002</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>100</v>
@@ -1300,7 +1308,7 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <f t="shared" si="0"/>
-        <v>1.2300000000000002</v>
+        <v>1.2500000000000002</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>101</v>
@@ -1309,7 +1317,7 @@
     <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <f t="shared" si="0"/>
-        <v>1.2400000000000002</v>
+        <v>1.2600000000000002</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>102</v>
@@ -1330,7 +1338,7 @@
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <f t="shared" si="0"/>
-        <v>1.2500000000000002</v>
+        <v>1.2700000000000002</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>23</v>
@@ -1345,7 +1353,7 @@
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <f t="shared" si="0"/>
-        <v>1.2600000000000002</v>
+        <v>1.2800000000000002</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>26</v>
@@ -1360,7 +1368,7 @@
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <f t="shared" si="0"/>
-        <v>1.2700000000000002</v>
+        <v>1.2900000000000003</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>29</v>
@@ -1381,7 +1389,7 @@
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <f t="shared" si="0"/>
-        <v>1.2800000000000002</v>
+        <v>1.3000000000000003</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>31</v>
@@ -1396,7 +1404,7 @@
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <f t="shared" si="0"/>
-        <v>1.2900000000000003</v>
+        <v>1.3100000000000003</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>33</v>
@@ -1417,7 +1425,7 @@
     <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <f t="shared" si="0"/>
-        <v>1.3000000000000003</v>
+        <v>1.3200000000000003</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>36</v>
@@ -1432,7 +1440,7 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <f t="shared" si="0"/>
-        <v>1.3100000000000003</v>
+        <v>1.3300000000000003</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>39</v>
@@ -1447,7 +1455,7 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <f t="shared" si="0"/>
-        <v>1.3200000000000003</v>
+        <v>1.3400000000000003</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>42</v>
@@ -1468,7 +1476,7 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <f t="shared" si="0"/>
-        <v>1.3300000000000003</v>
+        <v>1.3500000000000003</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>44</v>
@@ -1483,7 +1491,7 @@
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <f t="shared" si="0"/>
-        <v>1.3400000000000003</v>
+        <v>1.3600000000000003</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>42</v>
@@ -1498,7 +1506,7 @@
     <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <f t="shared" si="0"/>
-        <v>1.3500000000000003</v>
+        <v>1.3700000000000003</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>46</v>
@@ -1513,7 +1521,7 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <f t="shared" si="0"/>
-        <v>1.3600000000000003</v>
+        <v>1.3800000000000003</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>49</v>
@@ -1528,7 +1536,7 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <f t="shared" si="0"/>
-        <v>1.3700000000000003</v>
+        <v>1.3900000000000003</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>42</v>
@@ -1537,7 +1545,7 @@
         <v>43</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E41" s="2">
         <v>18</v>
@@ -1549,7 +1557,7 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <f t="shared" si="0"/>
-        <v>1.3800000000000003</v>
+        <v>1.4000000000000004</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>53</v>
@@ -1564,7 +1572,7 @@
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <f t="shared" si="0"/>
-        <v>1.3900000000000003</v>
+        <v>1.4100000000000004</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>42</v>
@@ -1573,13 +1581,13 @@
         <v>43</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <f t="shared" si="0"/>
-        <v>1.4000000000000004</v>
+        <v>1.4200000000000004</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>105</v>
@@ -1594,13 +1602,13 @@
     <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <f t="shared" si="0"/>
-        <v>1.4100000000000004</v>
+        <v>1.4300000000000004</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>107</v>
@@ -1622,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56F8A38-754B-4400-802D-2F35A96FA0FF}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,76 +1677,92 @@
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
+        <f>A2+0.01</f>
         <v>2.0099999999999998</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A26" si="0">A3+0.01</f>
+        <v>2.0199999999999996</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0299999999999994</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="1" t="s">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0399999999999991</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0499999999999989</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0599999999999987</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="E8" s="2">
         <v>14</v>
@@ -1748,15 +1772,18 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0699999999999985</v>
+      </c>
       <c r="B9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="E9" s="2">
         <v>6</v>
@@ -1766,27 +1793,33 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0799999999999983</v>
+      </c>
       <c r="B10" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D10" s="1" t="s">
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0899999999999981</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E11" s="2">
         <v>12</v>
@@ -1796,81 +1829,99 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0999999999999979</v>
+      </c>
       <c r="B12" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <f t="shared" si="0"/>
+        <v>2.1099999999999977</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <f t="shared" si="0"/>
+        <v>2.1199999999999974</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <f t="shared" si="0"/>
+        <v>2.1299999999999972</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <f t="shared" si="0"/>
+        <v>2.139999999999997</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>143</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="A17" s="3">
+        <f t="shared" si="0"/>
+        <v>2.1499999999999968</v>
+      </c>
       <c r="B17" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E17" s="2">
         <v>10</v>
@@ -1880,38 +1931,48 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="3">
+        <f t="shared" si="0"/>
+        <v>2.1599999999999966</v>
+      </c>
       <c r="B18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <f t="shared" si="0"/>
+        <v>2.1699999999999964</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <f t="shared" si="0"/>
+        <v>2.1799999999999962</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="D20" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E20" s="2">
         <v>13</v>
@@ -1921,36 +1982,48 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <f t="shared" si="0"/>
+        <v>2.1899999999999959</v>
+      </c>
       <c r="B21" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <f t="shared" si="0"/>
+        <v>2.1999999999999957</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2099999999999955</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="D23" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E23" s="2">
         <v>15</v>
@@ -1960,36 +2033,48 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2199999999999953</v>
+      </c>
       <c r="B24" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2299999999999951</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
+      <c r="D25" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2399999999999949</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E26" s="2">
         <v>8</v>

</xml_diff>